<commit_message>
corrigiendo carga de polizas
</commit_message>
<xml_diff>
--- a/APP PRINCIPAL/Modulos/MdRenovaciones/WVEPF106.xlsx
+++ b/APP PRINCIPAL/Modulos/MdRenovaciones/WVEPF106.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LeonelAlbertoMadridF\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7E509AB-57B6-4431-B05A-07489143825F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="20730" windowHeight="9540"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -477,8 +483,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -520,6 +526,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -568,7 +577,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -600,9 +609,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -634,6 +661,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -809,12 +854,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BK15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:BK10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="BA1" workbookViewId="0">
+      <selection activeCell="BK10" sqref="BK10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="58" max="58" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="59" max="59" width="42.140625" bestFit="1" customWidth="1"/>
@@ -822,7 +869,7 @@
     <col min="61" max="61" width="106.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:63">
+    <row r="1" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1013,7 +1060,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="2" spans="1:63">
+    <row r="2" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>91</v>
       </c>
@@ -1204,7 +1251,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:63">
+    <row r="3" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>91</v>
       </c>
@@ -1395,7 +1442,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:63">
+    <row r="4" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>91</v>
       </c>
@@ -1586,7 +1633,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="5" spans="1:63">
+    <row r="5" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>91</v>
       </c>
@@ -1777,7 +1824,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="6" spans="1:63">
+    <row r="6" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>91</v>
       </c>
@@ -1968,7 +2015,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="7" spans="1:63">
+    <row r="7" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>91</v>
       </c>
@@ -2159,7 +2206,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="8" spans="1:63">
+    <row r="8" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>91</v>
       </c>
@@ -2350,7 +2397,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="9" spans="1:63">
+    <row r="9" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>91</v>
       </c>
@@ -2541,7 +2588,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="10" spans="1:63">
+    <row r="10" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>91</v>
       </c>
@@ -2731,86 +2778,6 @@
       <c r="BK10" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="11" spans="1:63">
-      <c r="E11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
-      <c r="AV11" s="1"/>
-      <c r="AX11" s="1"/>
-      <c r="BB11" s="1"/>
-      <c r="BC11" s="1"/>
-      <c r="BD11" s="1"/>
-      <c r="BE11" s="1"/>
-    </row>
-    <row r="12" spans="1:63">
-      <c r="E12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
-      <c r="AV12" s="1"/>
-      <c r="AX12" s="1"/>
-      <c r="BB12" s="1"/>
-      <c r="BC12" s="1"/>
-      <c r="BD12" s="1"/>
-      <c r="BE12" s="1"/>
-    </row>
-    <row r="13" spans="1:63">
-      <c r="E13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
-      <c r="O13" s="1"/>
-      <c r="AV13" s="1"/>
-      <c r="AX13" s="1"/>
-      <c r="BB13" s="1"/>
-      <c r="BC13" s="1"/>
-      <c r="BD13" s="1"/>
-      <c r="BE13" s="1"/>
-    </row>
-    <row r="14" spans="1:63">
-      <c r="E14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
-      <c r="O14" s="1"/>
-      <c r="AV14" s="1"/>
-      <c r="AX14" s="1"/>
-      <c r="BB14" s="1"/>
-      <c r="BC14" s="1"/>
-      <c r="BD14" s="1"/>
-      <c r="BE14" s="1"/>
-    </row>
-    <row r="15" spans="1:63">
-      <c r="E15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
-      <c r="N15" s="1"/>
-      <c r="O15" s="1"/>
-      <c r="AV15" s="1"/>
-      <c r="AX15" s="1"/>
-      <c r="BB15" s="1"/>
-      <c r="BC15" s="1"/>
-      <c r="BD15" s="1"/>
-      <c r="BE15" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2819,24 +2786,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>